<commit_message>
Sales Report First Stage Completed
</commit_message>
<xml_diff>
--- a/Other/Populate Data.xlsx
+++ b/Other/Populate Data.xlsx
@@ -5,20 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\db-capstone-project-\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D00FFD-083E-4EB1-B229-8DC1D524E7C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717A50E6-4344-41D4-99DE-65DD9806B671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
     <sheet name="Employees" sheetId="2" r:id="rId2"/>
     <sheet name="Bookings" sheetId="4" r:id="rId3"/>
     <sheet name="Menu" sheetId="3" r:id="rId4"/>
-    <sheet name="Orders" sheetId="5" r:id="rId5"/>
-    <sheet name="Delivery" sheetId="7" r:id="rId6"/>
+    <sheet name="Menu Items" sheetId="8" r:id="rId5"/>
+    <sheet name="Orders" sheetId="5" r:id="rId6"/>
+    <sheet name="Delivery" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="326">
   <si>
     <t>CustomerID</t>
   </si>
@@ -661,42 +662,6 @@
     <t>(30, '2021-06-05', 7, 'C12', 'E1')</t>
   </si>
   <si>
-    <t>(1, 'Greek', 'Greek yoghurt', 6)</t>
-  </si>
-  <si>
-    <t>(2, 'Greek', 'Greek salad', 7)</t>
-  </si>
-  <si>
-    <t>(3, 'Greek', 'Olives', 10)</t>
-  </si>
-  <si>
-    <t>(4, 'Greek', 'Athens White wine', 13)</t>
-  </si>
-  <si>
-    <t>(5, 'Italian', 'Pizza', 12)</t>
-  </si>
-  <si>
-    <t>(6, 'Italian', 'Minestrone', 11)</t>
-  </si>
-  <si>
-    <t>(7, 'Italian', 'Corfu Red Wine', 21)</t>
-  </si>
-  <si>
-    <t>(8, 'Italian', 'Cheesecake', 13)</t>
-  </si>
-  <si>
-    <t>(9, 'Turkish', 'Turkish Coffee', 7)</t>
-  </si>
-  <si>
-    <t>(10, 'Turkish', 'Falafel', 17)</t>
-  </si>
-  <si>
-    <t>(11, 'Turkish', 'Ice cream', 15)</t>
-  </si>
-  <si>
-    <t>(12, 'Turkish', 'Hummus', 11)</t>
-  </si>
-  <si>
     <t>(1, '2022-09-20', 3, 30, 3, 21)</t>
   </si>
   <si>
@@ -968,6 +933,93 @@
   </si>
   <si>
     <t>('C15', 'Adolpho De Emanuele', 8486297)</t>
+  </si>
+  <si>
+    <t>ItemID</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Starter</t>
+  </si>
+  <si>
+    <t>Main Courses</t>
+  </si>
+  <si>
+    <t>Desserts</t>
+  </si>
+  <si>
+    <t>(1, 'Greek yoghurt', 'Starter', 6)</t>
+  </si>
+  <si>
+    <t>(2, 'Greek salad', 'Starter', 7)</t>
+  </si>
+  <si>
+    <t>(3, 'Olives', 'Main Courses', 10)</t>
+  </si>
+  <si>
+    <t>(4, 'Athens White wine', 'Desserts', 13)</t>
+  </si>
+  <si>
+    <t>(5, 'Pizza', 'Main Courses', 12)</t>
+  </si>
+  <si>
+    <t>(6, 'Minestrone', 'Starter', 11)</t>
+  </si>
+  <si>
+    <t>(7, 'Corfu Red Wine', 'Starter', 21)</t>
+  </si>
+  <si>
+    <t>(8, 'Cheesecake', 'Main Courses', 13)</t>
+  </si>
+  <si>
+    <t>(9, 'Turkish Coffee', 'Desserts', 7)</t>
+  </si>
+  <si>
+    <t>(10, 'Falafel', 'Starter', 17)</t>
+  </si>
+  <si>
+    <t>(11, 'Ice cream', 'Starter', 15)</t>
+  </si>
+  <si>
+    <t>(12, 'Hummus', 'Main Courses', 11)</t>
+  </si>
+  <si>
+    <t>(1, 1, 'Greek')</t>
+  </si>
+  <si>
+    <t>(1, 2, 'Greek')</t>
+  </si>
+  <si>
+    <t>(1, 3, 'Greek')</t>
+  </si>
+  <si>
+    <t>(1, 4, 'Greek')</t>
+  </si>
+  <si>
+    <t>(2, 5, 'Italian')</t>
+  </si>
+  <si>
+    <t>(2, 6, 'Italian')</t>
+  </si>
+  <si>
+    <t>(2, 7, 'Italian')</t>
+  </si>
+  <si>
+    <t>(2, 8, 'Italian')</t>
+  </si>
+  <si>
+    <t>(3, 9, 'Turkish')</t>
+  </si>
+  <si>
+    <t>(3, 10, 'Turkish')</t>
+  </si>
+  <si>
+    <t>(3, 11, 'Turkish')</t>
+  </si>
+  <si>
+    <t>(3, 12, 'Turkish')</t>
   </si>
 </sst>
 </file>
@@ -1016,27 +1068,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1325,8 +1357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1375,7 +1407,7 @@
         <v>('C1', 'Rowe Maciaszek', 4203493)</v>
       </c>
       <c r="G2" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -1397,7 +1429,7 @@
         <v>('C2', 'Saree MacGilfoyle', 4516885)</v>
       </c>
       <c r="G3" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -1419,7 +1451,7 @@
         <v>('C3', 'Brinn McCullum', 1251464)</v>
       </c>
       <c r="G4" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -1441,7 +1473,7 @@
         <v>('C4', 'Rowena Theobold', 5108826)</v>
       </c>
       <c r="G5" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -1463,7 +1495,7 @@
         <v>('C5', 'Aldin Wendover', 2186652)</v>
       </c>
       <c r="G6" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -1485,7 +1517,7 @@
         <v>('C6', 'Julie Tallyn', 3228539)</v>
       </c>
       <c r="G7" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -1507,7 +1539,7 @@
         <v>('C7', 'Xaviera Du Plantier', 2687532)</v>
       </c>
       <c r="G8" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -1529,7 +1561,7 @@
         <v>('C8', 'Nanette Trinkwon', 1167555)</v>
       </c>
       <c r="G9" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -1551,7 +1583,7 @@
         <v>('C9', 'Karena Jenicke', 8338349)</v>
       </c>
       <c r="G10" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -1573,7 +1605,7 @@
         <v>('C10', 'Nicolle Lardge', 9476459)</v>
       </c>
       <c r="G11" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -1595,7 +1627,7 @@
         <v>('C11', 'Willabella Farlambe', 6785267)</v>
       </c>
       <c r="G12" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -1617,7 +1649,7 @@
         <v>('C12', 'Idalina Prudence', 3755652)</v>
       </c>
       <c r="G13" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -1639,7 +1671,7 @@
         <v>('C13', 'Katey Methuen', 6024510)</v>
       </c>
       <c r="G14" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -1661,7 +1693,7 @@
         <v>('C14', 'Trixie Queen', 6245809)</v>
       </c>
       <c r="G15" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -1669,7 +1701,7 @@
         <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="C16">
         <v>8486297662</v>
@@ -1683,7 +1715,7 @@
         <v>('C15', 'Adolpho De Emanuele', 8486297)</v>
       </c>
       <c r="G16" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -1907,7 +1939,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2674,13 +2706,14 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.7265625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2690,13 +2723,13 @@
         <v>70</v>
       </c>
       <c r="B1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
         <v>52</v>
-      </c>
-      <c r="C1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D1" t="s">
-        <v>54</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>159</v>
@@ -2709,252 +2742,252 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>55</v>
       </c>
-      <c r="C2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2">
-        <v>6</v>
-      </c>
       <c r="E2" s="1" t="str">
-        <f>_xlfn.CONCAT("(", A2, ", ", "'", B2, "'", ", ", "'", C2, "'", ", ", D2, ")")</f>
-        <v>(1, 'Greek', 'Greek yoghurt', 6)</v>
+        <f>_xlfn.CONCAT("(", A2, ", ", B2,", ", "'",D2, "'",")")</f>
+        <v>(1, 1, 'Greek')</v>
       </c>
       <c r="G2" t="s">
-        <v>206</v>
+        <v>314</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>55</v>
       </c>
-      <c r="C3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3">
-        <v>7</v>
-      </c>
       <c r="E3" s="1" t="str">
-        <f t="shared" ref="E3:E13" si="0">_xlfn.CONCAT("(", A3, ", ", "'", B3, "'", ", ", "'", C3, "'", ", ", D3, ")")</f>
-        <v>(2, 'Greek', 'Greek salad', 7)</v>
+        <f>_xlfn.CONCAT("(", A3, ", ", B3,", ", "'",D3, "'",")")</f>
+        <v>(1, 2, 'Greek')</v>
       </c>
       <c r="G3" t="s">
-        <v>207</v>
+        <v>315</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
         <v>55</v>
       </c>
-      <c r="C4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
       <c r="E4" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(3, 'Greek', 'Olives', 10)</v>
+        <f>_xlfn.CONCAT("(", A4, ", ", B4,", ", "'",D4, "'",")")</f>
+        <v>(1, 3, 'Greek')</v>
       </c>
       <c r="G4" t="s">
-        <v>208</v>
+        <v>316</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
         <v>55</v>
       </c>
-      <c r="C5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5">
-        <v>13</v>
-      </c>
       <c r="E5" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(4, 'Greek', 'Athens White wine', 13)</v>
+        <f>_xlfn.CONCAT("(", A5, ", ", B5,", ", "'",D5, "'",")")</f>
+        <v>(1, 4, 'Greek')</v>
       </c>
       <c r="G5" t="s">
-        <v>209</v>
+        <v>317</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
         <v>60</v>
       </c>
-      <c r="C6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6">
-        <v>12</v>
-      </c>
       <c r="E6" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(5, 'Italian', 'Pizza', 12)</v>
+        <f>_xlfn.CONCAT("(", A6, ", ", B6,", ", "'",D6, "'",")")</f>
+        <v>(2, 5, 'Italian')</v>
       </c>
       <c r="G6" t="s">
-        <v>210</v>
+        <v>318</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
         <v>60</v>
       </c>
-      <c r="C7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7">
-        <v>11</v>
-      </c>
       <c r="E7" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(6, 'Italian', 'Minestrone', 11)</v>
+        <f>_xlfn.CONCAT("(", A7, ", ", B7,", ", "'",D7, "'",")")</f>
+        <v>(2, 6, 'Italian')</v>
       </c>
       <c r="G7" t="s">
-        <v>211</v>
+        <v>319</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
         <v>60</v>
       </c>
-      <c r="C8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8">
-        <v>21</v>
-      </c>
       <c r="E8" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(7, 'Italian', 'Corfu Red Wine', 21)</v>
+        <f>_xlfn.CONCAT("(", A8, ", ", B8,", ", "'",D8, "'",")")</f>
+        <v>(2, 7, 'Italian')</v>
       </c>
       <c r="G8" t="s">
-        <v>212</v>
+        <v>320</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
         <v>60</v>
       </c>
-      <c r="C9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9">
-        <v>13</v>
-      </c>
       <c r="E9" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(8, 'Italian', 'Cheesecake', 13)</v>
+        <f>_xlfn.CONCAT("(", A9, ", ", B9,", ", "'",D9, "'",")")</f>
+        <v>(2, 8, 'Italian')</v>
       </c>
       <c r="G9" t="s">
-        <v>213</v>
+        <v>321</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
         <v>65</v>
       </c>
-      <c r="C10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10">
-        <v>7</v>
-      </c>
       <c r="E10" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(9, 'Turkish', 'Turkish Coffee', 7)</v>
+        <f>_xlfn.CONCAT("(", A10, ", ", B10,", ", "'",D10, "'",")")</f>
+        <v>(3, 9, 'Turkish')</v>
       </c>
       <c r="G10" t="s">
-        <v>214</v>
+        <v>322</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
         <v>65</v>
       </c>
-      <c r="C11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11">
-        <v>17</v>
-      </c>
       <c r="E11" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(10, 'Turkish', 'Falafel', 17)</v>
+        <f>_xlfn.CONCAT("(", A11, ", ", B11,", ", "'",D11, "'",")")</f>
+        <v>(3, 10, 'Turkish')</v>
       </c>
       <c r="G11" t="s">
-        <v>215</v>
+        <v>323</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
         <v>65</v>
       </c>
-      <c r="C12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12">
-        <v>15</v>
-      </c>
       <c r="E12" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(11, 'Turkish', 'Ice cream', 15)</v>
+        <f>_xlfn.CONCAT("(", A12, ", ", B12,", ", "'",D12, "'",")")</f>
+        <v>(3, 11, 'Turkish')</v>
       </c>
       <c r="G12" t="s">
-        <v>216</v>
+        <v>324</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
         <v>65</v>
       </c>
-      <c r="C13" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13">
-        <v>11</v>
-      </c>
       <c r="E13" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>(12, 'Turkish', 'Hummus', 11)</v>
+        <f>_xlfn.CONCAT("(", A13, ", ", B13,", ", "'",D13, "'",")")</f>
+        <v>(3, 12, 'Turkish')</v>
       </c>
       <c r="G13" t="s">
-        <v>217</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -2963,11 +2996,305 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F9BF65A-9998-44AC-86AA-BE46E561B9D2}">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6328125" customWidth="1"/>
+    <col min="5" max="5" width="30.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="str">
+        <f>_xlfn.CONCAT("(", A2, ", ", "'",B2, "'", ", ", "'", C2, "'", ", ", D2, ")")</f>
+        <v>(1, 'Greek yoghurt', 'Starter', 6)</v>
+      </c>
+      <c r="G2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
+        <v>299</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="str">
+        <f t="shared" ref="E3:E13" si="0">_xlfn.CONCAT("(", A3, ", ", "'",B3, "'", ", ", "'", C3, "'", ", ", D3, ")")</f>
+        <v>(2, 'Greek salad', 'Starter', 7)</v>
+      </c>
+      <c r="G3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>300</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(3, 'Olives', 'Main Courses', 10)</v>
+      </c>
+      <c r="G4" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" t="s">
+        <v>301</v>
+      </c>
+      <c r="D5">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(4, 'Athens White wine', 'Desserts', 13)</v>
+      </c>
+      <c r="G5" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" t="s">
+        <v>300</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(5, 'Pizza', 'Main Courses', 12)</v>
+      </c>
+      <c r="G6" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" t="s">
+        <v>299</v>
+      </c>
+      <c r="D7">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(6, 'Minestrone', 'Starter', 11)</v>
+      </c>
+      <c r="G7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" t="s">
+        <v>299</v>
+      </c>
+      <c r="D8">
+        <v>21</v>
+      </c>
+      <c r="E8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(7, 'Corfu Red Wine', 'Starter', 21)</v>
+      </c>
+      <c r="G8" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
+        <v>300</v>
+      </c>
+      <c r="D9">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(8, 'Cheesecake', 'Main Courses', 13)</v>
+      </c>
+      <c r="G9" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" t="s">
+        <v>301</v>
+      </c>
+      <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(9, 'Turkish Coffee', 'Desserts', 7)</v>
+      </c>
+      <c r="G10" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" t="s">
+        <v>299</v>
+      </c>
+      <c r="D11">
+        <v>17</v>
+      </c>
+      <c r="E11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(10, 'Falafel', 'Starter', 17)</v>
+      </c>
+      <c r="G11" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" t="s">
+        <v>299</v>
+      </c>
+      <c r="D12">
+        <v>15</v>
+      </c>
+      <c r="E12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(11, 'Ice cream', 'Starter', 15)</v>
+      </c>
+      <c r="G12" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" t="s">
+        <v>300</v>
+      </c>
+      <c r="D13">
+        <v>11</v>
+      </c>
+      <c r="E13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(12, 'Hummus', 'Main Courses', 11)</v>
+      </c>
+      <c r="G13" t="s">
+        <v>313</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC42A82C-0034-43D7-A6F3-1DBF5F9A45F0}">
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2996,7 +3323,7 @@
         <v>107</v>
       </c>
       <c r="E1" t="s">
-        <v>70</v>
+        <v>297</v>
       </c>
       <c r="F1" t="s">
         <v>71</v>
@@ -3032,7 +3359,7 @@
         <v>(1, '2022-09-20', 3, 30, 3, 21)</v>
       </c>
       <c r="I2" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -3055,11 +3382,11 @@
         <v>25</v>
       </c>
       <c r="G3" s="1" t="str">
-        <f t="shared" ref="G3:G49" si="0">_xlfn.CONCAT("(", A3, ", ", "'", B3, "'", ", ", C3, ", ", D3, ", ", E3, ", ", F3, ")")</f>
+        <f>_xlfn.CONCAT("(", A3, ", ", "'", B3, "'", ", ", C3, ", ", D3, ", ", E3, ", ", F3, ")")</f>
         <v>(2, '2023-06-25', 7, 49, 2, 25)</v>
       </c>
       <c r="I3" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -3082,11 +3409,11 @@
         <v>13</v>
       </c>
       <c r="G4" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A4, ", ", "'", B4, "'", ", ", C4, ", ", D4, ", ", E4, ", ", F4, ")")</f>
         <v>(3, '2021-03-02', 2, 14, 2, 13)</v>
       </c>
       <c r="I4" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -3109,11 +3436,11 @@
         <v>15</v>
       </c>
       <c r="G5" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A5, ", ", "'", B5, "'", ", ", C5, ", ", D5, ", ", E5, ", ", F5, ")")</f>
         <v>(4, '2022-08-07', 5, 60, 5, 15)</v>
       </c>
       <c r="I5" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -3136,11 +3463,11 @@
         <v>29</v>
       </c>
       <c r="G6" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A6, ", ", "'", B6, "'", ", ", C6, ", ", D6, ", ", E6, ", ", F6, ")")</f>
         <v>(5, '2023-05-28', 1, 12, 5, 29)</v>
       </c>
       <c r="I6" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -3163,11 +3490,11 @@
         <v>15</v>
       </c>
       <c r="G7" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A7, ", ", "'", B7, "'", ", ", C7, ", ", D7, ", ", E7, ", ", F7, ")")</f>
         <v>(6, '2022-06-05', 4, 24, 1, 15)</v>
       </c>
       <c r="I7" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -3190,11 +3517,11 @@
         <v>3</v>
       </c>
       <c r="G8" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A8, ", ", "'", B8, "'", ", ", C8, ", ", D8, ", ", E8, ", ", F8, ")")</f>
         <v>(7, '2022-07-10', 6, 60, 3, 3)</v>
       </c>
       <c r="I8" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -3217,11 +3544,11 @@
         <v>26</v>
       </c>
       <c r="G9" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A9, ", ", "'", B9, "'", ", ", C9, ", ", D9, ", ", E9, ", ", F9, ")")</f>
         <v>(8, '2022-11-01', 2, 22, 12, 26)</v>
       </c>
       <c r="I9" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -3244,11 +3571,11 @@
         <v>10</v>
       </c>
       <c r="G10" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A10, ", ", "'", B10, "'", ", ", C10, ", ", D10, ", ", E10, ", ", F10, ")")</f>
         <v>(9, '2022-12-25', 7, 70, 3, 10)</v>
       </c>
       <c r="I10" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -3271,11 +3598,11 @@
         <v>7</v>
       </c>
       <c r="G11" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A11, ", ", "'", B11, "'", ", ", C11, ", ", D11, ", ", E11, ", ", F11, ")")</f>
         <v>(10, '2022-03-05', 2, 26, 4, 7)</v>
       </c>
       <c r="I11" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -3298,11 +3625,11 @@
         <v>19</v>
       </c>
       <c r="G12" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A12, ", ", "'", B12, "'", ", ", C12, ", ", D12, ", ", E12, ", ", F12, ")")</f>
         <v>(11, '2021-10-13', 5, 35, 2, 19)</v>
       </c>
       <c r="I12" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -3325,11 +3652,11 @@
         <v>2</v>
       </c>
       <c r="G13" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A13, ", ", "'", B13, "'", ", ", C13, ", ", D13, ", ", E13, ", ", F13, ")")</f>
         <v>(12, '2023-06-13', 7, 77, 12, 2)</v>
       </c>
       <c r="I13" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -3352,11 +3679,11 @@
         <v>8</v>
       </c>
       <c r="G14" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A14, ", ", "'", B14, "'", ", ", C14, ", ", D14, ", ", E14, ", ", F14, ")")</f>
         <v>(13, '2023-01-27', 5, 35, 2, 8)</v>
       </c>
       <c r="I14" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -3379,11 +3706,11 @@
         <v>23</v>
       </c>
       <c r="G15" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A15, ", ", "'", B15, "'", ", ", C15, ", ", D15, ", ", E15, ", ", F15, ")")</f>
         <v>(14, '2023-11-29', 1, 17, 10, 23)</v>
       </c>
       <c r="I15" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -3406,11 +3733,11 @@
         <v>13</v>
       </c>
       <c r="G16" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A16, ", ", "'", B16, "'", ", ", C16, ", ", D16, ", ", E16, ", ", F16, ")")</f>
         <v>(15, '2022-09-26', 3, 21, 2, 13)</v>
       </c>
       <c r="I16" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -3433,11 +3760,11 @@
         <v>15</v>
       </c>
       <c r="G17" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A17, ", ", "'", B17, "'", ", ", C17, ", ", D17, ", ", E17, ", ", F17, ")")</f>
         <v>(16, '2022-08-20', 2, 42, 7, 15)</v>
       </c>
       <c r="I17" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -3460,11 +3787,11 @@
         <v>26</v>
       </c>
       <c r="G18" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A18, ", ", "'", B18, "'", ", ", C18, ", ", D18, ", ", E18, ", ", F18, ")")</f>
         <v>(17, '2021-07-21', 5, 30, 1, 26)</v>
       </c>
       <c r="I18" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -3487,11 +3814,11 @@
         <v>2</v>
       </c>
       <c r="G19" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A19, ", ", "'", B19, "'", ", ", C19, ", ", D19, ", ", E19, ", ", F19, ")")</f>
         <v>(18, '2021-08-22', 1, 6, 1, 2)</v>
       </c>
       <c r="I19" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -3514,11 +3841,11 @@
         <v>15</v>
       </c>
       <c r="G20" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A20, ", ", "'", B20, "'", ", ", C20, ", ", D20, ", ", E20, ", ", F20, ")")</f>
         <v>(19, '2022-10-28', 3, 39, 8, 15)</v>
       </c>
       <c r="I20" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -3541,11 +3868,11 @@
         <v>17</v>
       </c>
       <c r="G21" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A21, ", ", "'", B21, "'", ", ", C21, ", ", D21, ", ", E21, ", ", F21, ")")</f>
         <v>(20, '2023-05-16', 2, 20, 3, 17)</v>
       </c>
       <c r="I21" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
@@ -3568,11 +3895,11 @@
         <v>14</v>
       </c>
       <c r="G22" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A22, ", ", "'", B22, "'", ", ", C22, ", ", D22, ", ", E22, ", ", F22, ")")</f>
         <v>(21, '2022-03-25', 2, 34, 10, 14)</v>
       </c>
       <c r="I22" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -3595,11 +3922,11 @@
         <v>9</v>
       </c>
       <c r="G23" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A23, ", ", "'", B23, "'", ", ", C23, ", ", D23, ", ", E23, ", ", F23, ")")</f>
         <v>(22, '2023-12-06', 4, 40, 3, 9)</v>
       </c>
       <c r="I23" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
@@ -3622,11 +3949,11 @@
         <v>3</v>
       </c>
       <c r="G24" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A24, ", ", "'", B24, "'", ", ", C24, ", ", D24, ", ", E24, ", ", F24, ")")</f>
         <v>(23, '2022-07-12', 2, 30, 11, 3)</v>
       </c>
       <c r="I24" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
@@ -3649,11 +3976,11 @@
         <v>28</v>
       </c>
       <c r="G25" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A25, ", ", "'", B25, "'", ", ", C25, ", ", D25, ", ", E25, ", ", F25, ")")</f>
         <v>(24, '2023-02-27', 3, 63, 7, 28)</v>
       </c>
       <c r="I25" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -3676,11 +4003,11 @@
         <v>16</v>
       </c>
       <c r="G26" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A26, ", ", "'", B26, "'", ", ", C26, ", ", D26, ", ", E26, ", ", F26, ")")</f>
         <v>(25, '2022-07-11', 6, 42, 9, 16)</v>
       </c>
       <c r="I26" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
@@ -3703,11 +4030,11 @@
         <v>20</v>
       </c>
       <c r="G27" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A27, ", ", "'", B27, "'", ", ", C27, ", ", D27, ", ", E27, ", ", F27, ")")</f>
         <v>(26, '2023-03-14', 1, 13, 4, 20)</v>
       </c>
       <c r="I27" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
@@ -3730,11 +4057,11 @@
         <v>15</v>
       </c>
       <c r="G28" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A28, ", ", "'", B28, "'", ", ", C28, ", ", D28, ", ", E28, ", ", F28, ")")</f>
         <v>(27, '2021-10-18', 4, 52, 4, 15)</v>
       </c>
       <c r="I28" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
@@ -3757,11 +4084,11 @@
         <v>2</v>
       </c>
       <c r="G29" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A29, ", ", "'", B29, "'", ", ", C29, ", ", D29, ", ", E29, ", ", F29, ")")</f>
         <v>(28, '2023-11-08', 6, 36, 1, 2)</v>
       </c>
       <c r="I29" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
@@ -3784,11 +4111,11 @@
         <v>8</v>
       </c>
       <c r="G30" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A30, ", ", "'", B30, "'", ", ", C30, ", ", D30, ", ", E30, ", ", F30, ")")</f>
         <v>(29, '2023-06-30', 1, 17, 10, 8)</v>
       </c>
       <c r="I30" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
@@ -3811,11 +4138,11 @@
         <v>15</v>
       </c>
       <c r="G31" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A31, ", ", "'", B31, "'", ", ", C31, ", ", D31, ", ", E31, ", ", F31, ")")</f>
         <v>(30, '2022-07-23', 7, 91, 8, 15)</v>
       </c>
       <c r="I31" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
@@ -3838,11 +4165,11 @@
         <v>7</v>
       </c>
       <c r="G32" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A32, ", ", "'", B32, "'", ", ", C32, ", ", D32, ", ", E32, ", ", F32, ")")</f>
         <v>(31, '2022-03-31', 5, 65, 4, 7)</v>
       </c>
       <c r="I32" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
@@ -3865,11 +4192,11 @@
         <v>27</v>
       </c>
       <c r="G33" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A33, ", ", "'", B33, "'", ", ", C33, ", ", D33, ", ", E33, ", ", F33, ")")</f>
         <v>(32, '2022-06-28', 1, 7, 9, 27)</v>
       </c>
       <c r="I33" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
@@ -3892,11 +4219,11 @@
         <v>19</v>
       </c>
       <c r="G34" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A34, ", ", "'", B34, "'", ", ", C34, ", ", D34, ", ", E34, ", ", F34, ")")</f>
         <v>(33, '2022-11-28', 2, 22, 6, 19)</v>
       </c>
       <c r="I34" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
@@ -3919,11 +4246,11 @@
         <v>27</v>
       </c>
       <c r="G35" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A35, ", ", "'", B35, "'", ", ", C35, ", ", D35, ", ", E35, ", ", F35, ")")</f>
         <v>(34, '2021-01-25', 3, 30, 3, 27)</v>
       </c>
       <c r="I35" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
@@ -3946,11 +4273,11 @@
         <v>4</v>
       </c>
       <c r="G36" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A36, ", ", "'", B36, "'", ", ", C36, ", ", D36, ", ", E36, ", ", F36, ")")</f>
         <v>(35, '2023-11-16', 4, 24, 1, 4)</v>
       </c>
       <c r="I36" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
@@ -3973,11 +4300,11 @@
         <v>3</v>
       </c>
       <c r="G37" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A37, ", ", "'", B37, "'", ", ", C37, ", ", D37, ", ", E37, ", ", F37, ")")</f>
         <v>(36, '2022-06-04', 5, 30, 1, 3)</v>
       </c>
       <c r="I37" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
@@ -4000,11 +4327,11 @@
         <v>7</v>
       </c>
       <c r="G38" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A38, ", ", "'", B38, "'", ", ", C38, ", ", D38, ", ", E38, ", ", F38, ")")</f>
         <v>(37, '2023-06-25', 5, 55, 6, 7)</v>
       </c>
       <c r="I38" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
@@ -4027,11 +4354,11 @@
         <v>15</v>
       </c>
       <c r="G39" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A39, ", ", "'", B39, "'", ", ", C39, ", ", D39, ", ", E39, ", ", F39, ")")</f>
         <v>(38, '2023-05-06', 3, 18, 1, 15)</v>
       </c>
       <c r="I39" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
@@ -4054,11 +4381,11 @@
         <v>26</v>
       </c>
       <c r="G40" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A40, ", ", "'", B40, "'", ", ", C40, ", ", D40, ", ", E40, ", ", F40, ")")</f>
         <v>(39, '2022-07-08', 6, 42, 2, 26)</v>
       </c>
       <c r="I40" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
@@ -4081,11 +4408,11 @@
         <v>11</v>
       </c>
       <c r="G41" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A41, ", ", "'", B41, "'", ", ", C41, ", ", D41, ", ", E41, ", ", F41, ")")</f>
         <v>(40, '2022-12-17', 4, 24, 1, 11)</v>
       </c>
       <c r="I41" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
@@ -4108,11 +4435,11 @@
         <v>17</v>
       </c>
       <c r="G42" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A42, ", ", "'", B42, "'", ", ", C42, ", ", D42, ", ", E42, ", ", F42, ")")</f>
         <v>(41, '2022-08-31', 5, 85, 10, 17)</v>
       </c>
       <c r="I42" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
@@ -4135,11 +4462,11 @@
         <v>26</v>
       </c>
       <c r="G43" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A43, ", ", "'", B43, "'", ", ", C43, ", ", D43, ", ", E43, ", ", F43, ")")</f>
         <v>(42, '2022-08-01', 2, 22, 6, 26)</v>
       </c>
       <c r="I43" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
@@ -4162,11 +4489,11 @@
         <v>26</v>
       </c>
       <c r="G44" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A44, ", ", "'", B44, "'", ", ", C44, ", ", D44, ", ", E44, ", ", F44, ")")</f>
         <v>(43, '2023-07-25', 2, 22, 12, 26)</v>
       </c>
       <c r="I44" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
@@ -4189,11 +4516,11 @@
         <v>13</v>
       </c>
       <c r="G45" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A45, ", ", "'", B45, "'", ", ", C45, ", ", D45, ", ", E45, ", ", F45, ")")</f>
         <v>(44, '2023-02-11', 1, 10, 3, 13)</v>
       </c>
       <c r="I45" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
@@ -4216,11 +4543,11 @@
         <v>14</v>
       </c>
       <c r="G46" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A46, ", ", "'", B46, "'", ", ", C46, ", ", D46, ", ", E46, ", ", F46, ")")</f>
         <v>(45, '2021-08-13', 7, 119, 10, 14)</v>
       </c>
       <c r="I46" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
@@ -4243,11 +4570,11 @@
         <v>4</v>
       </c>
       <c r="G47" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A47, ", ", "'", B47, "'", ", ", C47, ", ", D47, ", ", E47, ", ", F47, ")")</f>
         <v>(46, '2022-04-22', 5, 75, 11, 4)</v>
       </c>
       <c r="I47" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
@@ -4270,11 +4597,11 @@
         <v>16</v>
       </c>
       <c r="G48" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A48, ", ", "'", B48, "'", ", ", C48, ", ", D48, ", ", E48, ", ", F48, ")")</f>
         <v>(47, '2021-01-07', 1, 21, 7, 16)</v>
       </c>
       <c r="I48" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
@@ -4297,27 +4624,27 @@
         <v>22</v>
       </c>
       <c r="G49" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("(", A49, ", ", "'", B49, "'", ", ", C49, ", ", D49, ", ", E49, ", ", F49, ")")</f>
         <v>(48, '2022-02-03', 7, 77, 6, 22)</v>
       </c>
       <c r="I49" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K2:K28">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9858823-8C25-44D8-BBD6-E8EEEDF6245F}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4364,11 +4691,11 @@
         <v>156</v>
       </c>
       <c r="E2" s="1" t="str">
-        <f>_xlfn.CONCAT("(", A2, ", ", B2, ", ", "'",C2,"'", ", ", "'", D2, "'", ")")</f>
+        <f t="shared" ref="E2:E28" si="0">_xlfn.CONCAT("(", A2, ", ", B2, ", ", "'",C2,"'", ", ", "'", D2, "'", ")")</f>
         <v>(1, 7, '2022-07-10', 'Ready To Deliver')</v>
       </c>
       <c r="G2" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -4385,11 +4712,11 @@
         <v>158</v>
       </c>
       <c r="E3" s="1" t="str">
-        <f>_xlfn.CONCAT("(", A3, ", ", B3, ", ", "'",C3,"'", ", ", "'", D3, "'", ")")</f>
+        <f t="shared" si="0"/>
         <v>(2, 47, '2021-01-07', 'In Progress')</v>
       </c>
       <c r="G3" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -4406,11 +4733,11 @@
         <v>158</v>
       </c>
       <c r="E4" s="1" t="str">
-        <f>_xlfn.CONCAT("(", A4, ", ", B4, ", ", "'",C4,"'", ", ", "'", D4, "'", ")")</f>
+        <f t="shared" si="0"/>
         <v>(3, 38, '2023-05-06', 'In Progress')</v>
       </c>
       <c r="G4" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -4427,11 +4754,11 @@
         <v>157</v>
       </c>
       <c r="E5" s="1" t="str">
-        <f>_xlfn.CONCAT("(", A5, ", ", B5, ", ", "'",C5,"'", ", ", "'", D5, "'", ")")</f>
+        <f t="shared" si="0"/>
         <v>(4, 34, '2021-01-25', 'Delivered')</v>
       </c>
       <c r="G5" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -4448,11 +4775,11 @@
         <v>156</v>
       </c>
       <c r="E6" s="1" t="str">
-        <f>_xlfn.CONCAT("(", A6, ", ", B6, ", ", "'",C6,"'", ", ", "'", D6, "'", ")")</f>
+        <f t="shared" si="0"/>
         <v>(5, 46, '2022-04-22', 'Ready To Deliver')</v>
       </c>
       <c r="G6" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -4469,11 +4796,11 @@
         <v>157</v>
       </c>
       <c r="E7" s="1" t="str">
-        <f>_xlfn.CONCAT("(", A7, ", ", B7, ", ", "'",C7,"'", ", ", "'", D7, "'", ")")</f>
+        <f t="shared" si="0"/>
         <v>(6, 35, '2023-11-16', 'Delivered')</v>
       </c>
       <c r="G7" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -4490,11 +4817,11 @@
         <v>158</v>
       </c>
       <c r="E8" s="1" t="str">
-        <f>_xlfn.CONCAT("(", A8, ", ", B8, ", ", "'",C8,"'", ", ", "'", D8, "'", ")")</f>
+        <f t="shared" si="0"/>
         <v>(7, 18, '2021-08-22', 'In Progress')</v>
       </c>
       <c r="G8" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -4511,11 +4838,11 @@
         <v>156</v>
       </c>
       <c r="E9" s="1" t="str">
-        <f>_xlfn.CONCAT("(", A9, ", ", B9, ", ", "'",C9,"'", ", ", "'", D9, "'", ")")</f>
+        <f t="shared" si="0"/>
         <v>(8, 6, '2022-06-05', 'Ready To Deliver')</v>
       </c>
       <c r="G9" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -4532,11 +4859,11 @@
         <v>158</v>
       </c>
       <c r="E10" s="1" t="str">
-        <f>_xlfn.CONCAT("(", A10, ", ", B10, ", ", "'",C10,"'", ", ", "'", D10, "'", ")")</f>
+        <f t="shared" si="0"/>
         <v>(9, 40, '2022-12-17', 'In Progress')</v>
       </c>
       <c r="G10" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -4553,11 +4880,11 @@
         <v>157</v>
       </c>
       <c r="E11" s="1" t="str">
-        <f>_xlfn.CONCAT("(", A11, ", ", B11, ", ", "'",C11,"'", ", ", "'", D11, "'", ")")</f>
+        <f t="shared" si="0"/>
         <v>(10, 31, '2022-03-31', 'Delivered')</v>
       </c>
       <c r="G11" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -4574,11 +4901,11 @@
         <v>156</v>
       </c>
       <c r="E12" s="1" t="str">
-        <f>_xlfn.CONCAT("(", A12, ", ", B12, ", ", "'",C12,"'", ", ", "'", D12, "'", ")")</f>
+        <f t="shared" si="0"/>
         <v>(11, 5, '2023-05-28', 'Ready To Deliver')</v>
       </c>
       <c r="G12" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -4595,11 +4922,11 @@
         <v>158</v>
       </c>
       <c r="E13" s="1" t="str">
-        <f>_xlfn.CONCAT("(", A13, ", ", B13, ", ", "'",C13,"'", ", ", "'", D13, "'", ")")</f>
+        <f t="shared" si="0"/>
         <v>(12, 48, '2022-02-03', 'In Progress')</v>
       </c>
       <c r="G13" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -4616,11 +4943,11 @@
         <v>156</v>
       </c>
       <c r="E14" s="1" t="str">
-        <f>_xlfn.CONCAT("(", A14, ", ", B14, ", ", "'",C14,"'", ", ", "'", D14, "'", ")")</f>
+        <f t="shared" si="0"/>
         <v>(13, 41, '2022-08-31', 'Ready To Deliver')</v>
       </c>
       <c r="G14" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -4637,11 +4964,11 @@
         <v>156</v>
       </c>
       <c r="E15" s="1" t="str">
-        <f>_xlfn.CONCAT("(", A15, ", ", B15, ", ", "'",C15,"'", ", ", "'", D15, "'", ")")</f>
+        <f t="shared" si="0"/>
         <v>(14, 39, '2022-07-08', 'Ready To Deliver')</v>
       </c>
       <c r="G15" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -4658,11 +4985,11 @@
         <v>157</v>
       </c>
       <c r="E16" s="1" t="str">
-        <f>_xlfn.CONCAT("(", A16, ", ", B16, ", ", "'",C16,"'", ", ", "'", D16, "'", ")")</f>
+        <f t="shared" si="0"/>
         <v>(15, 25, '2022-07-11', 'Delivered')</v>
       </c>
       <c r="G16" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -4679,11 +5006,11 @@
         <v>157</v>
       </c>
       <c r="E17" s="1" t="str">
-        <f>_xlfn.CONCAT("(", A17, ", ", B17, ", ", "'",C17,"'", ", ", "'", D17, "'", ")")</f>
+        <f t="shared" si="0"/>
         <v>(16, 26, '2023-03-14', 'Delivered')</v>
       </c>
       <c r="G17" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -4700,11 +5027,11 @@
         <v>157</v>
       </c>
       <c r="E18" s="1" t="str">
-        <f>_xlfn.CONCAT("(", A18, ", ", B18, ", ", "'",C18,"'", ", ", "'", D18, "'", ")")</f>
+        <f t="shared" si="0"/>
         <v>(17, 8, '2022-11-01', 'Delivered')</v>
       </c>
       <c r="G18" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -4721,11 +5048,11 @@
         <v>156</v>
       </c>
       <c r="E19" s="1" t="str">
-        <f>_xlfn.CONCAT("(", A19, ", ", B19, ", ", "'",C19,"'", ", ", "'", D19, "'", ")")</f>
+        <f t="shared" si="0"/>
         <v>(18, 17, '2021-07-21', 'Ready To Deliver')</v>
       </c>
       <c r="G19" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -4742,11 +5069,11 @@
         <v>156</v>
       </c>
       <c r="E20" s="1" t="str">
-        <f>_xlfn.CONCAT("(", A20, ", ", B20, ", ", "'",C20,"'", ", ", "'", D20, "'", ")")</f>
+        <f t="shared" si="0"/>
         <v>(19, 14, '2023-11-29', 'Ready To Deliver')</v>
       </c>
       <c r="G20" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -4763,11 +5090,11 @@
         <v>156</v>
       </c>
       <c r="E21" s="1" t="str">
-        <f>_xlfn.CONCAT("(", A21, ", ", B21, ", ", "'",C21,"'", ", ", "'", D21, "'", ")")</f>
+        <f t="shared" si="0"/>
         <v>(20, 36, '2022-06-04', 'Ready To Deliver')</v>
       </c>
       <c r="G21" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -4784,11 +5111,11 @@
         <v>157</v>
       </c>
       <c r="E22" s="1" t="str">
-        <f>_xlfn.CONCAT("(", A22, ", ", B22, ", ", "'",C22,"'", ", ", "'", D22, "'", ")")</f>
+        <f t="shared" si="0"/>
         <v>(21, 9, '2022-12-25', 'Delivered')</v>
       </c>
       <c r="G22" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -4805,11 +5132,11 @@
         <v>157</v>
       </c>
       <c r="E23" s="1" t="str">
-        <f>_xlfn.CONCAT("(", A23, ", ", B23, ", ", "'",C23,"'", ", ", "'", D23, "'", ")")</f>
+        <f t="shared" si="0"/>
         <v>(22, 19, '2022-10-28', 'Delivered')</v>
       </c>
       <c r="G23" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -4826,11 +5153,11 @@
         <v>156</v>
       </c>
       <c r="E24" s="1" t="str">
-        <f>_xlfn.CONCAT("(", A24, ", ", B24, ", ", "'",C24,"'", ", ", "'", D24, "'", ")")</f>
+        <f t="shared" si="0"/>
         <v>(23, 11, '2021-10-13', 'Ready To Deliver')</v>
       </c>
       <c r="G24" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -4847,11 +5174,11 @@
         <v>156</v>
       </c>
       <c r="E25" s="1" t="str">
-        <f>_xlfn.CONCAT("(", A25, ", ", B25, ", ", "'",C25,"'", ", ", "'", D25, "'", ")")</f>
+        <f t="shared" si="0"/>
         <v>(24, 44, '2023-02-11', 'Ready To Deliver')</v>
       </c>
       <c r="G25" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
@@ -4868,11 +5195,11 @@
         <v>158</v>
       </c>
       <c r="E26" s="1" t="str">
-        <f>_xlfn.CONCAT("(", A26, ", ", B26, ", ", "'",C26,"'", ", ", "'", D26, "'", ")")</f>
+        <f t="shared" si="0"/>
         <v>(25, 21, '2022-03-25', 'In Progress')</v>
       </c>
       <c r="G26" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
@@ -4889,11 +5216,11 @@
         <v>156</v>
       </c>
       <c r="E27" s="1" t="str">
-        <f>_xlfn.CONCAT("(", A27, ", ", B27, ", ", "'",C27,"'", ", ", "'", D27, "'", ")")</f>
+        <f t="shared" si="0"/>
         <v>(26, 3, '2021-03-02', 'Ready To Deliver')</v>
       </c>
       <c r="G27" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
@@ -4910,11 +5237,11 @@
         <v>156</v>
       </c>
       <c r="E28" s="1" t="str">
-        <f>_xlfn.CONCAT("(", A28, ", ", B28, ", ", "'",C28,"'", ", ", "'", D28, "'", ")")</f>
+        <f t="shared" si="0"/>
         <v>(27, 29, '2023-06-30', 'Ready To Deliver')</v>
       </c>
       <c r="G28" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>